<commit_message>
flat master at org-year level
</commit_message>
<xml_diff>
--- a/Raw Data (dont edit)/Ranking of GFC inputs.xlsx
+++ b/Raw Data (dont edit)/Ranking of GFC inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bednarek\Dropbox (Global Fund)\Public\Grantmaking\Knowledge\Datakind\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcarder\Documents\Dev\GFC\Raw Data (dont edit)\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FFB246-CF70-4C5F-9F21-66E9A8098BA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Rank</t>
   </si>
@@ -32,34 +33,40 @@
     <t>GFC input</t>
   </si>
   <si>
-    <t xml:space="preserve">Leveraging </t>
-  </si>
-  <si>
     <t>Monitoring Site Visit</t>
   </si>
   <si>
     <t>Knowledge Exchange Participation</t>
   </si>
   <si>
-    <t>Grantee Partner-Led Convening Participation</t>
-  </si>
-  <si>
     <t>Phone Call</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Legal Referral</t>
   </si>
   <si>
     <t>Meeting that is not a site visit or at a KE</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Site Visit</t>
+  </si>
+  <si>
+    <t>Additional Touch</t>
+  </si>
+  <si>
+    <t>Leveraging</t>
+  </si>
+  <si>
+    <t>Grantee-Led Convening Participation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,20 +398,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -412,47 +419,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -460,20 +467,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>